<commit_message>
Trying to link events to speaker pages
</commit_message>
<xml_diff>
--- a/docs/events.xlsx
+++ b/docs/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saiem 70\Desktop\Summer 2021 projects\DIFA\R_codes\hello_world\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\git\difa-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1C7890-3BB0-4663-B0A7-12E9C56E0B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6654BD82-921B-4C8C-815F-A25389A360DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
     <t>[Tim Beatty](https://are.ucdavis.edu/people/faculty/tim-beatty/)</t>
   </si>
   <si>
-    <t>[Julia Lane](https://wagner.nyu.edu/community/faculty/julia-lane)</t>
-  </si>
-  <si>
     <t>[Julia Lane](https://wagner.nyu.edu/community/faculty/julia-lane), [Jason Owen-Smith](https://lsa.umich.edu/soc/people/faculty/jdos.html)</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>Closing from the FAMPS and FSN Chairs; Preview of Day 2</t>
+  </si>
+  <si>
+    <t>[Julia Lane](https://dataifa.github.io/difa-project/julia_lane.html)</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +511,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -531,7 +531,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
         <v>34</v>
@@ -574,7 +574,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -594,7 +594,7 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -614,7 +614,7 @@
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -654,7 +654,7 @@
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
         <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -691,7 +691,7 @@
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Linking leadership team to events
</commit_message>
<xml_diff>
--- a/docs/events.xlsx
+++ b/docs/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\git\difa-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B83ABE-8F6E-4DD4-851F-7FA212391D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBE8358-1BB4-46DC-8497-BF7D352EB450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58380" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,12 +129,6 @@
     <t>60 minutes</t>
   </si>
   <si>
-    <t>[Lauren Chenarides](https://wpcarey.asu.edu/people/profile/3153292), [Drew Hanks](https://ehe.osu.edu/human-sciences/directory?id=hanks.46)</t>
-  </si>
-  <si>
-    <t>[Andi Carlson](https://www.ers.usda.gov/authors/ers-staff-directory/andrea-carlson/)</t>
-  </si>
-  <si>
     <t>[Ayaz Hyder](https://cph.osu.edu/people/ahyder), [Charlotte Ambrozek](https://are.ucdavis.edu/people/grad-students/phd/charlotte-ambrozek/)</t>
   </si>
   <si>
@@ -157,6 +151,12 @@
   </si>
   <si>
     <t>[Tim Beatty](https://dataifa.github.io/difa-project/timothy_beatty.html)</t>
+  </si>
+  <si>
+    <t>[Lauren Chenarides](https://dataifa.github.io/difa-project/Leadership_team.html), [Drew Hanks](https://dataifa.github.io/difa-project/Leadership_team.html)</t>
+  </si>
+  <si>
+    <t>[Andi Carlson](https://dataifa.github.io/difa-project/Leadership_team.html)</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +511,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -531,10 +531,10 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -554,7 +554,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -574,7 +574,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -594,7 +594,7 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -614,7 +614,7 @@
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -654,7 +654,7 @@
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
         <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -691,10 +691,10 @@
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating leadership bios take 2
</commit_message>
<xml_diff>
--- a/docs/events.xlsx
+++ b/docs/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\git\difa-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBE8358-1BB4-46DC-8497-BF7D352EB450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FC6EDB-C751-4A76-875A-D40E19154301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>[Tim Beatty](https://dataifa.github.io/difa-project/timothy_beatty.html)</t>
   </si>
   <si>
-    <t>[Lauren Chenarides](https://dataifa.github.io/difa-project/Leadership_team.html), [Drew Hanks](https://dataifa.github.io/difa-project/Leadership_team.html)</t>
-  </si>
-  <si>
-    <t>[Andi Carlson](https://dataifa.github.io/difa-project/Leadership_team.html)</t>
+    <t>[Lauren Chenarides](https://dataifa.github.io/difa-project/lauren_chenarides.html), [Drew Hanks](https://dataifa.github.io/difa-project/drew_hanks.html)</t>
+  </si>
+  <si>
+    <t>[Andi Carlson](https://dataifa.github.io/difa-project/andi_carlson.html)</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
trying to make stubs stick
</commit_message>
<xml_diff>
--- a/docs/events.xlsx
+++ b/docs/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\git\difa-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43136262-0039-43D4-B8D4-B489B8284AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097D922D-9A87-4880-A320-F8508477ACED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33240" yWindow="2025" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
updating events2 and slides
</commit_message>
<xml_diff>
--- a/docs/events.xlsx
+++ b/docs/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\git\difa-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F3EEF3-0DDF-4C0F-AF87-46D05BB4E5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6535818B-2E34-4690-9B5C-5FC9FD9475E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31005" yWindow="2025" windowWidth="24255" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>